<commit_message>
[REPO] Código para replicar lineas de pobreza CONEVAL
</commit_message>
<xml_diff>
--- a/06_replicando_lineas_pobreza/equivalencia_enigh_inpc.xlsx
+++ b/06_replicando_lineas_pobreza/equivalencia_enigh_inpc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgejuvenalcamposferreira/Desktop/MCV/Encargo 54. Canastas/archivos_replica_lineas_pobreza/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57A9A40-6102-964B-ABA9-379196084A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8373997-FA52-9C41-A2BF-620C684D153B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="3900" windowWidth="28040" windowHeight="17440" xr2:uid="{637B6C8F-27D7-CF44-9018-384C93A3A8A2}"/>
+    <workbookView xWindow="33180" yWindow="4560" windowWidth="28040" windowHeight="17440" xr2:uid="{637B6C8F-27D7-CF44-9018-384C93A3A8A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2352,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C57FADC-042A-B64E-AF67-B5D71361C4B2}">
   <dimension ref="A1:D383"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>